<commit_message>
allow to change type of entity
</commit_message>
<xml_diff>
--- a/data/edited-entities.xlsx
+++ b/data/edited-entities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/birk/Documents/Jobs/SAPA/Development/pellaton-experience-data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF27D13B-C81D-8B41-A20A-57AACD8A9AFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C140D5E3-A129-8E4B-AF07-40E63C6BDE4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38680" windowHeight="31360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5920" yWindow="880" windowWidth="38680" windowHeight="31360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="entities" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="996" uniqueCount="675">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="998" uniqueCount="675">
   <si>
     <t>name</t>
   </si>
@@ -2337,7 +2337,7 @@
   </sheetPr>
   <dimension ref="A1:Z314"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E78" sqref="E78"/>
     </sheetView>
@@ -6269,11 +6269,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EED1A47-D285-DB40-BAF6-24A9377E1F76}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6305,6 +6305,14 @@
         <v>7</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:C2" xr:uid="{84520EBE-AB57-6F41-95BA-B108393683E4}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6317,7 +6325,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:A1048576"/>
+      <selection pane="bottomLeft" activeCell="F72" sqref="F72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>